<commit_message>
actualizar boton categoria seleccion
</commit_message>
<xml_diff>
--- a/palabras_categorias.xlsx
+++ b/palabras_categorias.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,21 +508,6 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>2025-03-06 15:52:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>TRABAJO</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-03-06 18:24:32</t>
         </is>
       </c>
     </row>
@@ -537,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,7 +570,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -606,7 +591,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -627,7 +612,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -669,7 +654,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -711,7 +696,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -774,7 +759,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -879,7 +864,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -1005,7 +990,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1026,7 +1011,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1052,6 +1037,48 @@
       <c r="E24" t="inlineStr">
         <is>
           <t>2025-03-06 16:53:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>guineo</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:42:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:53:22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
integracion IA a juego 2
</commit_message>
<xml_diff>
--- a/palabras_categorias.xlsx
+++ b/palabras_categorias.xlsx
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>

</xml_diff>